<commit_message>
working script, only from localhost and only for new user
</commit_message>
<xml_diff>
--- a/users-creator/examples/excel.xlsx
+++ b/users-creator/examples/excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samuel/EPFL/Biot/tools/users-creator/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D6C51A9-FB00-8F43-A00A-C59F7EB6EC29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2246A4CA-11C5-FF4C-A1C4-84660BA2558A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{345AA04F-B42B-5143-968F-05FF6E902C33}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>username</t>
   </si>
@@ -52,6 +52,21 @@
   </si>
   <si>
     <t>password_2</t>
+  </si>
+  <si>
+    <t>user_id</t>
+  </si>
+  <si>
+    <t>user1</t>
+  </si>
+  <si>
+    <t>user2</t>
+  </si>
+  <si>
+    <t>company</t>
+  </si>
+  <si>
+    <t>script</t>
   </si>
 </sst>
 </file>
@@ -484,20 +499,24 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
+      <c r="D1" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
@@ -509,7 +528,13 @@
         <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>2</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -517,7 +542,13 @@
         <v>4</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>5</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
remove company from the excel
</commit_message>
<xml_diff>
--- a/users-creator/examples/excel.xlsx
+++ b/users-creator/examples/excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samuel/EPFL/Biot/tools/users-creator/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2246A4CA-11C5-FF4C-A1C4-84660BA2558A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFAEC167-9014-3442-8B88-3DDCD028610F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{345AA04F-B42B-5143-968F-05FF6E902C33}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>username</t>
   </si>
@@ -61,12 +61,6 @@
   </si>
   <si>
     <t>user2</t>
-  </si>
-  <si>
-    <t>company</t>
-  </si>
-  <si>
-    <t>script</t>
   </si>
 </sst>
 </file>
@@ -107,7 +101,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -161,11 +155,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -182,6 +185,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -496,10 +506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEC67507-EC30-0445-A4BB-0825B1803F60}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -514,9 +524,7 @@
       <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>9</v>
-      </c>
+      <c r="D1" s="4"/>
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
@@ -530,12 +538,11 @@
       <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>10</v>
-      </c>
+      <c r="D2" s="6"/>
+      <c r="E2" s="8"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -544,12 +551,80 @@
       <c r="B3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>10</v>
-      </c>
+      <c r="D3" s="6"/>
+      <c r="E3" s="8"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D4" s="6"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D5" s="6"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D6" s="6"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D7" s="6"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D8" s="6"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D9" s="6"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D10" s="6"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D11" s="6"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D12" s="6"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D13" s="6"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D14" s="6"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D15" s="6"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D16" s="6"/>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D17" s="6"/>
+    </row>
+    <row r="18" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D18" s="6"/>
+    </row>
+    <row r="19" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D19" s="6"/>
+    </row>
+    <row r="20" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D20" s="6"/>
+    </row>
+    <row r="21" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D21" s="6"/>
+    </row>
+    <row r="22" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D22" s="6"/>
+    </row>
+    <row r="23" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D23" s="6"/>
+    </row>
+    <row r="24" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D24" s="6"/>
+    </row>
+    <row r="25" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D25" s="6"/>
+    </row>
+    <row r="26" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D26" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>